<commit_message>
Added the Acceptance TestPlan!
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\IdeaProjects\team-project-2185-swen-261-14-c-zug\etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DDEFA9-F84F-4A61-AB86-B04954FD891E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4320" windowWidth="18705" windowHeight="7545" tabRatio="500"/>
+    <workbookView xWindow="-3945" yWindow="1500" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,17 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Instructions</t>
   </si>
   <si>
-    <t>Team Name</t>
-  </si>
-  <si>
-    <t>Testing Team Name</t>
-  </si>
-  <si>
     <t>User Story</t>
   </si>
   <si>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>fill in when doing cross-team or Freshman Seminar testing</t>
-  </si>
-  <si>
-    <t>Your team name as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers</t>
   </si>
   <si>
     <t>Tester initials; date; comments (required if test failed)</t>
@@ -118,11 +112,1046 @@
 Save this test plan with a name formatted as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers.xslx.
 Submit this file per the instructions specified for the sprint submissions, cross-team testing, and Freshman Seminar testing.</t>
   </si>
+  <si>
+    <t>2185-swen-14-261-c Avoiding Zuggzwang</t>
+  </si>
+  <si>
+    <t>Start a Game (13)</t>
+  </si>
+  <si>
+    <t>Test results</t>
+  </si>
+  <si>
+    <t>pass! 2/24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that the player I selected isn't yet in a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I select that player </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the system will begin a checkers 
+game and assign me as the starting (Red) player and my opponent as the White player.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a valid, initial game board </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I view the board in the browser </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> my pieces are oriented on the bottom
+ of the board grid just like I would see the board if I were playing in the physical world.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">** that I'm signed in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I view the Home page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I can start a game by selecting a player listed on
+ the Home page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I'm waiting for a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> another player selects a game with me </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the system will automatically
+ send me to the _Game View_ as the White player.  _NOTE_: the `home.ftl` HTML includes a `&lt;meta&gt;` tag that tells the browser
+ to refresh the game every 5 seconds; thus you need to update the `GetHomeRoute` controller to handle the situation when a 
+player is assigned a game.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a valid, initial game board </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">I drag a piece to a white space </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the piece should </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+be _droppable_.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a valid, initial game board </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I view the board in the browser </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> my pieces are oriented 
+on the bottom of the board grid just like I would see the board if I were playing in the physical world.</t>
+    </r>
+  </si>
+  <si>
+    <t>Player Sign-in (8)</t>
+  </si>
+  <si>
+    <t>Initials of Testers</t>
+  </si>
+  <si>
+    <t>EN, AB, CB, TK, JJ</t>
+  </si>
+  <si>
+    <t>EN, AB, TK</t>
+  </si>
+  <si>
+    <t>EN, Ab, TK, CB</t>
+  </si>
+  <si>
+    <t>AB, TK, JJ</t>
+  </si>
+  <si>
+    <t>AB, CB, EN, TK, JJ</t>
+  </si>
+  <si>
+    <t>AB, CB, TK</t>
+  </si>
+  <si>
+    <t>TK, CB, JJ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I have not signed in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I see the Home page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I must see a means to sign-in. 
+(such as a link or button)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I am not signed-in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I do click on the sign-in link </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect to be taken to the Sign-in page, with 
+a means to enter a player name.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that no one else is using my name </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I enter my name containing at least one alphanumeric character and 
+optionally spaces in the sign-in form and click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign-in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect the system to reserve my name and
+ navigate back to the Home page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I am on the Sign-in page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I enter a name that does not contain at least one alphanumeric character 
+or contains one or more characters that are not alphanumeric or spaces and click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign-in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect the 
+system to reject this name and return the Sign-in page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that someone else with my name has signed-in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I enter my name in the Sign-in form and click the 
+**Sign-in** button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect the system to reject my sign-in and return the Sign-in page with a message for me 
+to try another name.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I am signed-in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I navigate to the Home page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect to see a list of all the other signed-in
+ players who are available to play a game.  (_NOTE_: in the next story you will use this list to pick opponents for checkers games.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I am signed-in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I navigate to the Home page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect to see a list of all the other
+ signed-in players who are available to play a game.  (_NOTE_: in the next story you will use this list to pick opponents for 
+checkers games.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I am _not_ signed-in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I navigate to the Home page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect to see a message of 
+how many players are signed-in but not a list of them (for privacy reasons).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -222,7 +1251,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -271,197 +1314,14 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -788,11 +1648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -801,32 +1661,199 @@
     <col min="2" max="2" width="106.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="79.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="79.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="48" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="48" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="48" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -836,7 +1863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H599"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -859,36 +1886,36 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="8"/>
       <c r="E2" s="8"/>
@@ -897,7 +1924,7 @@
     <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="8"/>
       <c r="E3" s="8"/>
@@ -906,7 +1933,7 @@
     <row r="4" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8"/>
       <c r="E4" s="8"/>
@@ -915,7 +1942,7 @@
     <row r="5" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="8"/>
       <c r="E5" s="8"/>
@@ -924,7 +1951,7 @@
     <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="8"/>
       <c r="E6" s="8"/>
@@ -933,7 +1960,7 @@
     <row r="7" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="8"/>
       <c r="E7" s="8"/>
@@ -942,7 +1969,7 @@
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="8"/>
       <c r="E8" s="8"/>
@@ -951,7 +1978,7 @@
     <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="8"/>
       <c r="E9" s="8"/>
@@ -960,7 +1987,7 @@
     <row r="10" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="8"/>
       <c r="E10" s="8"/>
@@ -968,10 +1995,10 @@
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="11"/>
@@ -983,7 +2010,7 @@
     <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="8"/>
       <c r="E12" s="8"/>
@@ -992,7 +2019,7 @@
     <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="8"/>
       <c r="E13" s="8"/>
@@ -1001,7 +2028,7 @@
     <row r="14" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="8"/>
       <c r="E14" s="8"/>
@@ -1010,7 +2037,7 @@
     <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="8"/>
       <c r="E15" s="8"/>
@@ -1019,7 +2046,7 @@
     <row r="16" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="8"/>
       <c r="E16" s="8"/>
@@ -1028,7 +2055,7 @@
     <row r="17" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="8"/>
       <c r="E17" s="8"/>
@@ -1037,7 +2064,7 @@
     <row r="18" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="8"/>
       <c r="E18" s="8"/>
@@ -3952,39 +4979,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C599 E2:E599 G2:G599">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D599">
-    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F599">
-    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H599">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E599 C2:C599 G2:G599">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E599 C2:C599 G2:G599" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated Acceptance Test Plan, Removed 2 todos
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\IdeaProjects\team-project-2185-swen-261-14-c-zug\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DDEFA9-F84F-4A61-AB86-B04954FD891E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FFEA79-4B51-4A40-9F82-A391B5BF0934}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3945" yWindow="1500" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="450" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
   <si>
     <t>Instructions</t>
   </si>
@@ -1147,12 +1147,891 @@
 how many players are signed-in but not a list of them (for privacy reasons).</t>
     </r>
   </si>
+  <si>
+    <t>Sign out (3)</t>
+  </si>
+  <si>
+    <r>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">** that I am on the sign out page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I confirm my decision to sign out **</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>** I expect to be returned to the 
+pre-sign in home page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>** that I am on the sign out page **</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>** I confirm that I want to sign out **</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>** I expect my data to be 
+removed from the server.</t>
+    </r>
+  </si>
+  <si>
+    <t>PASS! 3/26</t>
+  </si>
+  <si>
+    <t>EN, AB</t>
+  </si>
+  <si>
+    <r>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>** I am signed in as a player **</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>** click a 'sign out' link **</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>** I expect to be taken to a page where I
+ can confirm my choice to sign out.</t>
+    </r>
+  </si>
+  <si>
+    <t>Resignation (5)</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* I'm in a game *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* my opponent resigns *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* I expect to win.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I am in a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> either player resigns </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect to be returned to the home page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I'm in a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I resign </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect my opponent to win.</t>
+    </r>
+  </si>
+  <si>
+    <t>Simple Moves (8)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that my piece is not a King </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I make a simple move </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect to only be able to move one space diagonally forward</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I'm in a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I move my piece to a valid space </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect my piece to move to the given location.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it is my turn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I move to an invalid spot, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect my piece will not move</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I’m in a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it is not my turn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect that my piece will not move</t>
+    </r>
+  </si>
+  <si>
+    <t>EN, AB, TK CB JJ</t>
+  </si>
+  <si>
+    <t>EN, AB, TK, CB, JJ</t>
+  </si>
+  <si>
+    <t>Single Jump (5)</t>
+  </si>
+  <si>
+    <t>END OF SPRINT 1 SPRINT TWO BEGINNING</t>
+  </si>
+  <si>
+    <t>Given I’m in a game and it is my turn, when I jump over a piece, then I expect to capture that piece</t>
+  </si>
+  <si>
+    <t>Given I’m in a game and it is not my turn, when I jump over a piece, then I expect the move to not happen</t>
+  </si>
+  <si>
+    <t>Out of Pieces (8)</t>
+  </si>
+  <si>
+    <r>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">** a player is in a game **when** their last piece is captured </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect the game to end.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I am in a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I lost my last peice to either a regular jump or a super mega death jump </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+i expect to lose</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given I am a player</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I capture the last piece and submit the move </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect a win.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1180,6 +2059,14 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1211,7 +2098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1247,6 +2134,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1649,10 +2537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1818,7 +2706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="48" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>51</v>
       </c>
@@ -1829,7 +2717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="48" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="48" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>52</v>
       </c>
@@ -1840,7 +2728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="32.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>53</v>
       </c>
@@ -1849,6 +2737,145 @@
       </c>
       <c r="D19" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added unit testing to sign out route
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\IdeaProjects\team-project-2185-swen-261-14-c-zug\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FFEA79-4B51-4A40-9F82-A391B5BF0934}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47269F25-6065-4049-88F7-285DAF5E1B04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4275" yWindow="450" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
   <si>
     <t>Instructions</t>
   </si>
@@ -2025,6 +2025,34 @@
       </rPr>
       <t xml:space="preserve"> I expect a win.</t>
     </r>
+  </si>
+  <si>
+    <t>Super Mega Jump of Death (8)</t>
+  </si>
+  <si>
+    <t>Given I am in a game and it is my turn, when I leap over multiple pieces, then I expect to capture all of those pieces</t>
+  </si>
+  <si>
+    <t>Given I am in a game and it is my turn, when I try to leap over multiple pieces invalidly, then I expect the move not to happen</t>
+  </si>
+  <si>
+    <t>PASS 3/27</t>
+  </si>
+  <si>
+    <t>CB, EN, TK</t>
+  </si>
+  <si>
+    <t>Incomplete Testing, and logic not moved in. Decided to complete the project rather than move on with implementing this story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Pass  3/27</t>
+  </si>
+  <si>
+    <t>CB,EN,TK</t>
   </si>
 </sst>
 </file>
@@ -2537,10 +2565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2847,35 +2875,78 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B34" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B37" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added retrieved acceptence test plan
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\IdeaProjects\team-project-2185-swen-261-14-c-zug\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4719062E-C4B7-4700-BCCF-30C6D8ECDBE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3E1EC80-1B76-4602-AF05-44D79A3F53E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4275" yWindow="450" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="120">
   <si>
     <t>Instructions</t>
   </si>
@@ -2075,12 +2075,87 @@
   <si>
     <t>TK, EN, AB</t>
   </si>
+  <si>
+    <t xml:space="preserve">END OF SPRINT TWO SPRINT THREE BEGINNING </t>
+  </si>
+  <si>
+    <t>Finish Multi-Jump Validation (3)</t>
+  </si>
+  <si>
+    <t>Given I have started a multi-jump, when I attempt to submit without finishing the jump, I should see an error</t>
+  </si>
+  <si>
+    <t>Given I have completed a multi-jump, when I attempt to submit the finished multi-jump, then I expect the move to be valid</t>
+  </si>
+  <si>
+    <t>Out of moves (5)</t>
+  </si>
+  <si>
+    <t>**Given** that i am a player **when** my opponent or I cannot make a move **then** I EXPECT the game to end.</t>
+  </si>
+  <si>
+    <t>**Given** that the game ends **when** either player cannot make a move **then** I EXPECT the player who moved last to be the winner.</t>
+  </si>
+  <si>
+    <t>**Given** that the game ends **when** either player cannot make a move **then** I EXPECT the players to be informed that the game is over and who won.</t>
+  </si>
+  <si>
+    <t>**Given** that I am a player **when** it is my turn and I have available moves **then** I EXPECT the game to continue as normal</t>
+  </si>
+  <si>
+    <t>AI Move (5)</t>
+  </si>
+  <si>
+    <t>**Given** I play against AI **when** when the AI takes its turn **then** I expect the AI to follow the same rules</t>
+  </si>
+  <si>
+    <t>**Give** I play against an AI **when** it is its turn **then** I expect it to make a jump move when posible</t>
+  </si>
+  <si>
+    <t>Save Replay (3)</t>
+  </si>
+  <si>
+    <t>**Given** that I am in a game **when** it ends **then** I expect the server to save that game so that it can be watched latter</t>
+  </si>
+  <si>
+    <t>Enter Replay mode (5)</t>
+  </si>
+  <si>
+    <t>**Given** I am in the menu **when** I click enter replay mode **then** I EXPECT to be in replay mode and see my saved games.</t>
+  </si>
+  <si>
+    <t>Given that there is a replay saved when i click on replay mode then I expect to see a list of all the saved games</t>
+  </si>
+  <si>
+    <t>Watching Replay Mode (5)</t>
+  </si>
+  <si>
+    <t>**Given** I am in replay mode **when** I click on the next move button **then** I EXPECT to be able to see the result of the next turn.</t>
+  </si>
+  <si>
+    <t>Given I am in replay mode, when I click on the back up move button, then I expect to be able to see the previous state of the game</t>
+  </si>
+  <si>
+    <t>Forcing Jumps (5)</t>
+  </si>
+  <si>
+    <t>Given when I attempt to submit a simple turn when a jump is possible then I expect an error message</t>
+  </si>
+  <si>
+    <t>**Given** a player is in a game **when** their last piece is captured **then** I expect the game to end.</t>
+  </si>
+  <si>
+    <t>**Given** **when** I capture the last piece and submit the move *then* I expect a win.</t>
+  </si>
+  <si>
+    <t>**given** that I am in a game **When** I lost my last peice to either a regular jump or a super mega death jump **then** i expect to lose</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2117,6 +2192,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF17394D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2147,7 +2236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2184,6 +2273,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2586,10 +2677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3012,6 +3103,120 @@
       </c>
       <c r="D44" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A45" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Unit Testing to have all the STUFF that we have done
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\IdeaProjects\team-project-2185-swen-261-14-c-zug\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3E1EC80-1B76-4602-AF05-44D79A3F53E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45BD0213-1F29-45F2-860C-A5ED69A82C2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4275" yWindow="450" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="123">
   <si>
     <t>Instructions</t>
   </si>
@@ -2149,6 +2149,15 @@
   </si>
   <si>
     <t>**given** that I am in a game **When** I lost my last peice to either a regular jump or a super mega death jump **then** i expect to lose</t>
+  </si>
+  <si>
+    <t>Pass 4/10</t>
+  </si>
+  <si>
+    <t>TK, EN, CB</t>
+  </si>
+  <si>
+    <t>TK,EN,CB</t>
   </si>
 </sst>
 </file>
@@ -2679,8 +2688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3117,36 +3126,72 @@
       <c r="B46" t="s">
         <v>97</v>
       </c>
+      <c r="C46" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>99</v>
       </c>
       <c r="B49" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
@@ -3154,12 +3199,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>107</v>
       </c>
@@ -3167,7 +3212,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>109</v>
       </c>
@@ -3175,12 +3220,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>112</v>
       </c>
@@ -3188,35 +3233,67 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B64" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B66" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>120</v>
+      </c>
+      <c r="D66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>120</v>
+      </c>
+      <c r="D67" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>119</v>
+      </c>
+      <c r="C68" t="s">
+        <v>120</v>
+      </c>
+      <c r="D68" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Acceptance Test Plan excel file
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\IdeaProjects\team-project-2185-swen-261-14-c-zug\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3E1EC80-1B76-4602-AF05-44D79A3F53E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F903DF22-32D2-4107-A188-C705F89B157F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="450" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="129">
   <si>
     <t>Instructions</t>
   </si>
@@ -2149,6 +2149,33 @@
   </si>
   <si>
     <t>**given** that I am in a game **When** I lost my last peice to either a regular jump or a super mega death jump **then** i expect to lose</t>
+  </si>
+  <si>
+    <t>PASS 4/15</t>
+  </si>
+  <si>
+    <t>EN AB TK CB JJ</t>
+  </si>
+  <si>
+    <t>Pass 4/15</t>
+  </si>
+  <si>
+    <t>EN AB TK CB</t>
+  </si>
+  <si>
+    <t>CB, EN</t>
+  </si>
+  <si>
+    <t>EN, CB, AB, TK</t>
+  </si>
+  <si>
+    <t>EN,CB, AB, TK</t>
+  </si>
+  <si>
+    <t>EN, CB, TK,JJ, TK</t>
+  </si>
+  <si>
+    <t>EN,CB,TK,JJ</t>
   </si>
 </sst>
 </file>
@@ -2679,8 +2706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3117,106 +3144,208 @@
       <c r="B46" t="s">
         <v>97</v>
       </c>
+      <c r="C46" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>99</v>
       </c>
       <c r="B49" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B54" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B57" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B59" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>120</v>
+      </c>
+      <c r="D59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>120</v>
+      </c>
+      <c r="D60" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B61" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B64" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B66" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>122</v>
+      </c>
+      <c r="D66" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>122</v>
+      </c>
+      <c r="D67" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>119</v>
+      </c>
+      <c r="C68" t="s">
+        <v>122</v>
+      </c>
+      <c r="D68" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>